<commit_message>
✨ Update Rapport document and Scrum Master Report
</commit_message>
<xml_diff>
--- a/docs/GL/Scrum Master Report.xlsx
+++ b/docs/GL/Scrum Master Report.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26105"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="99" documentId="11_9248CACD84F5E813E97046798E3E8C1851038385" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CE9DA1B2-A585-4926-A4F3-49E80AA51878}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dylan\Documents\GitHub\gp-dam-teamflexsante\docs\GL\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D98489B-19AE-4599-91BE-F10E4D56463C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -28,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
   <si>
     <t>Assignee / Weeks</t>
   </si>
@@ -145,6 +150,18 @@
   </si>
   <si>
     <t>UC Insert Data</t>
+  </si>
+  <si>
+    <t>Create a Scrum Master Excel Report</t>
+  </si>
+  <si>
+    <t>Rework UC2 Sequence Diagrams</t>
+  </si>
+  <si>
+    <t>Create a Product Owner Excel Report</t>
+  </si>
+  <si>
+    <t>Add exceptions for UC1 Sequence Diagrams</t>
   </si>
 </sst>
 </file>
@@ -236,7 +253,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -353,13 +370,38 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -382,6 +424,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -400,7 +448,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -698,250 +746,283 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C3:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="3" width="16.140625" customWidth="1"/>
-    <col min="4" max="4" width="27.42578125" customWidth="1"/>
-    <col min="5" max="5" width="27.28515625" customWidth="1"/>
-    <col min="6" max="6" width="32.7109375" customWidth="1"/>
-    <col min="7" max="7" width="33.5703125" customWidth="1"/>
+    <col min="3" max="3" width="16.109375" customWidth="1"/>
+    <col min="4" max="4" width="27.44140625" customWidth="1"/>
+    <col min="5" max="5" width="27.33203125" customWidth="1"/>
+    <col min="6" max="6" width="32.6640625" customWidth="1"/>
+    <col min="7" max="7" width="33.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:7">
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="22">
+      <c r="D3" s="21">
         <v>44907</v>
       </c>
-      <c r="E3" s="22">
+      <c r="E3" s="21">
         <v>44929</v>
       </c>
-      <c r="F3" s="22">
+      <c r="F3" s="23">
         <v>44937</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="26">
         <v>44942</v>
       </c>
     </row>
     <row r="4" spans="3:7">
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="20" t="s">
         <v>4</v>
       </c>
+      <c r="G4" s="27" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="5" spans="3:7">
-      <c r="C5" s="20"/>
-      <c r="D5" s="18" t="s">
+      <c r="C5" s="19"/>
+      <c r="D5" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8" t="s">
+      <c r="E5" s="7"/>
+      <c r="F5" s="20" t="s">
         <v>3</v>
       </c>
+      <c r="G5" s="28" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="6" spans="3:7">
-      <c r="C6" s="20"/>
-      <c r="D6" s="18" t="s">
+      <c r="C6" s="19"/>
+      <c r="D6" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="28"/>
     </row>
     <row r="7" spans="3:7">
-      <c r="C7" s="20"/>
-      <c r="D7" s="8" t="s">
+      <c r="C7" s="19"/>
+      <c r="D7" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="28"/>
     </row>
     <row r="8" spans="3:7">
-      <c r="C8" s="20"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="28"/>
     </row>
     <row r="9" spans="3:7">
-      <c r="C9" s="20"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="28"/>
     </row>
     <row r="10" spans="3:7">
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8" t="s">
+      <c r="E10" s="7"/>
+      <c r="F10" s="20" t="s">
         <v>9</v>
       </c>
+      <c r="G10" s="28"/>
     </row>
     <row r="11" spans="3:7">
-      <c r="C11" s="13"/>
-      <c r="D11" s="16" t="s">
+      <c r="C11" s="12"/>
+      <c r="D11" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="28"/>
     </row>
     <row r="12" spans="3:7">
-      <c r="C12" s="13"/>
-      <c r="D12" s="16" t="s">
+      <c r="C12" s="12"/>
+      <c r="D12" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="28"/>
     </row>
     <row r="13" spans="3:7">
-      <c r="C13" s="13"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="28"/>
     </row>
     <row r="14" spans="3:7">
-      <c r="C14" s="13"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="28"/>
     </row>
     <row r="15" spans="3:7">
-      <c r="C15" s="13"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="28"/>
     </row>
     <row r="16" spans="3:7">
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="17" t="s">
+      <c r="D16" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="E16" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F16" s="8" t="s">
+      <c r="F16" s="20" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="3:6">
-      <c r="C17" s="13"/>
-      <c r="D17" s="17" t="s">
+      <c r="G16" s="28" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7">
+      <c r="C17" s="12"/>
+      <c r="D17" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="E17" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F17" s="8" t="s">
+      <c r="F17" s="20" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="18" spans="3:6">
-      <c r="C18" s="13"/>
-      <c r="D18" s="17" t="s">
+      <c r="G17" s="28" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7">
+      <c r="C18" s="12"/>
+      <c r="D18" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-    </row>
-    <row r="19" spans="3:6">
-      <c r="C19" s="13"/>
-      <c r="D19" s="9" t="s">
+      <c r="E18" s="7"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="28"/>
+    </row>
+    <row r="19" spans="3:7">
+      <c r="C19" s="12"/>
+      <c r="D19" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-    </row>
-    <row r="20" spans="3:6">
-      <c r="C20" s="13"/>
-      <c r="D20" s="9" t="s">
+      <c r="E19" s="7"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="28"/>
+    </row>
+    <row r="20" spans="3:7">
+      <c r="C20" s="12"/>
+      <c r="D20" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-    </row>
-    <row r="21" spans="3:6">
-      <c r="C21" s="13"/>
-      <c r="D21" s="23" t="s">
+      <c r="E20" s="7"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="28"/>
+    </row>
+    <row r="21" spans="3:7">
+      <c r="C21" s="12"/>
+      <c r="D21" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-    </row>
-    <row r="22" spans="3:6">
-      <c r="C22" s="13"/>
-      <c r="D22" s="8" t="s">
+      <c r="E21" s="10"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="28"/>
+    </row>
+    <row r="22" spans="3:7">
+      <c r="C22" s="12"/>
+      <c r="D22" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-    </row>
-    <row r="23" spans="3:6">
-      <c r="C23" s="13"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-    </row>
-    <row r="24" spans="3:6">
-      <c r="C24" s="13"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="11"/>
-    </row>
-    <row r="25" spans="3:6">
-      <c r="C25" s="12" t="s">
+      <c r="E22" s="7"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="28"/>
+    </row>
+    <row r="23" spans="3:7">
+      <c r="C23" s="12"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="28"/>
+    </row>
+    <row r="24" spans="3:7">
+      <c r="C24" s="12"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="28"/>
+    </row>
+    <row r="25" spans="3:7">
+      <c r="C25" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="D25" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E25" s="21" t="s">
+      <c r="E25" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="F25" s="8" t="s">
+      <c r="F25" s="20" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="3:6">
-      <c r="C26" s="13"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="14" t="s">
+      <c r="G25" s="28"/>
+    </row>
+    <row r="26" spans="3:7">
+      <c r="C26" s="12"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="25" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="3:6">
-      <c r="C27" s="13"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8" t="s">
+      <c r="G26" s="28"/>
+    </row>
+    <row r="27" spans="3:7">
+      <c r="C27" s="12"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="20" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="3:6">
-      <c r="C28" s="14"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-    </row>
-    <row r="35" spans="3:5" ht="18">
-      <c r="D35" s="2" t="s">
+      <c r="G27" s="28"/>
+    </row>
+    <row r="28" spans="3:7">
+      <c r="C28" s="13"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="28"/>
+    </row>
+    <row r="35" spans="3:5" ht="17.399999999999999">
+      <c r="D35" s="1" t="s">
         <v>27</v>
       </c>
     </row>
@@ -949,7 +1030,7 @@
       <c r="C36" t="s">
         <v>28</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="D36" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E36" t="s">
@@ -957,7 +1038,7 @@
       </c>
     </row>
     <row r="37" spans="3:5">
-      <c r="D37" s="4" t="s">
+      <c r="D37" s="3" t="s">
         <v>31</v>
       </c>
       <c r="E37" t="s">
@@ -965,7 +1046,7 @@
       </c>
     </row>
     <row r="38" spans="3:5">
-      <c r="D38" s="5" t="s">
+      <c r="D38" s="4" t="s">
         <v>33</v>
       </c>
       <c r="E38" t="s">
@@ -973,7 +1054,7 @@
       </c>
     </row>
     <row r="39" spans="3:5">
-      <c r="D39" s="6" t="s">
+      <c r="D39" s="5" t="s">
         <v>35</v>
       </c>
       <c r="E39" t="s">
@@ -981,7 +1062,7 @@
       </c>
     </row>
     <row r="40" spans="3:5">
-      <c r="D40" s="7" t="s">
+      <c r="D40" s="6" t="s">
         <v>37</v>
       </c>
       <c r="E40" t="s">

</xml_diff>